<commit_message>
Updated using test data from excel file. Added log out step in test 1 to run all tests of Login class.
</commit_message>
<xml_diff>
--- a/src/test/resources/input_data.xlsx
+++ b/src/test/resources/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bharatkammakatla/TestAutomation/SeleniumJavaFramework/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyle/IdeaProjects/fresherQELearn/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FCA8B3-22CB-F049-9291-C9AD4737F083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61E37A3-9FF4-194E-A675-4BD618FFBFFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2463F9C5-1750-0048-8FEB-74FF33B32275}"/>
+    <workbookView xWindow="8880" yWindow="6360" windowWidth="19920" windowHeight="11640" xr2:uid="{2463F9C5-1750-0048-8FEB-74FF33B32275}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,58 +25,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TCID</t>
   </si>
   <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>ThisIsNotAPassword</t>
-  </si>
-  <si>
-    <t>Facility</t>
-  </si>
-  <si>
-    <t>Hongkong CURA Healthcare Center</t>
-  </si>
-  <si>
-    <t>Visit Date</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>Test message: Regular check up</t>
-  </si>
-  <si>
     <t>TC1</t>
   </si>
   <si>
     <t>TC2</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>CURA Healthcare</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>invalidPassword</t>
+  </si>
+  <si>
+    <t>johndoe</t>
+  </si>
+  <si>
+    <t>validPassword1!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -98,12 +77,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -119,7 +92,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -127,14 +100,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745E163B-7AA0-DE48-B629-E9896DDF2F3D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,72 +449,40 @@
     <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1">
-        <v>44051</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>